<commit_message>
ID90project final push-Readme,ID90 updated
</commit_message>
<xml_diff>
--- a/ID90.xlsx
+++ b/ID90.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21255" windowHeight="8205"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21255" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -66,19 +66,19 @@
     <t>airline-email-3</t>
   </si>
   <si>
-    <t>Campo Search</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>id="destination"</t>
-  </si>
-  <si>
     <t>//*[@class='btn btn-primary text-uppercase gtm-get-started-btn']</t>
   </si>
   <si>
     <t>//*[@class='btn btn-link text-uppercase mt-3 font-weight-bold text-white d-lg-none']</t>
+  </si>
+  <si>
+    <t>Mensaje Contact us</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//*[@class='primary-content gtm-footer-link']</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -584,13 +584,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>